<commit_message>
agregar correo para Bancolom Davivien y CA, CC para bancolombia
</commit_message>
<xml_diff>
--- a/PAGOPROVEEDORES.xlsx
+++ b/PAGOPROVEEDORES.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Forero\Desktop\pago-proveedores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Forero\Desktop\Pago-proveedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CEC014-AA9E-48D0-B9B8-4F058C78835F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB2641F-E894-49BF-BCE0-9EF23DCB826C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="295">
   <si>
     <t>Tipo de Identificacion</t>
   </si>
@@ -918,6 +918,9 @@
   </si>
   <si>
     <t>DE COLOMBIA SA</t>
+  </si>
+  <si>
+    <t>51000000</t>
   </si>
 </sst>
 </file>
@@ -962,7 +965,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -972,6 +975,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1017,7 +1026,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1048,6 +1057,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1336,8 +1348,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:J291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G114" sqref="G114"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4413,7 +4425,7 @@
       <c r="J109" s="9"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="8">
+      <c r="A110" s="12">
         <v>1</v>
       </c>
       <c r="B110" s="8">
@@ -4425,9 +4437,15 @@
       <c r="D110" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E110" s="8"/>
-      <c r="F110" s="8"/>
-      <c r="G110" s="10"/>
+      <c r="E110" s="8">
+        <v>51</v>
+      </c>
+      <c r="F110" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G110" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="H110" s="6">
         <v>193970</v>
       </c>
@@ -4435,7 +4453,7 @@
       <c r="J110" s="9"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="8">
+      <c r="A111" s="12">
         <v>1</v>
       </c>
       <c r="B111" s="8">
@@ -4447,9 +4465,15 @@
       <c r="D111" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="E111" s="8"/>
-      <c r="F111" s="8"/>
-      <c r="G111" s="10"/>
+      <c r="E111" s="8">
+        <v>7</v>
+      </c>
+      <c r="F111" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G111" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="H111" s="6">
         <v>172500</v>
       </c>
@@ -4457,7 +4481,7 @@
       <c r="J111" s="9"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="8">
+      <c r="A112" s="12">
         <v>1</v>
       </c>
       <c r="B112" s="8">
@@ -4469,9 +4493,15 @@
       <c r="D112" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E112" s="8"/>
-      <c r="F112" s="8"/>
-      <c r="G112" s="10"/>
+      <c r="E112" s="8">
+        <v>7</v>
+      </c>
+      <c r="F112" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G112" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="H112" s="6">
         <v>1819546</v>
       </c>
@@ -4479,7 +4509,7 @@
       <c r="J112" s="9"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="8">
+      <c r="A113" s="12">
         <v>1</v>
       </c>
       <c r="B113" s="8">
@@ -4491,9 +4521,15 @@
       <c r="D113" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E113" s="8"/>
-      <c r="F113" s="8"/>
-      <c r="G113" s="10"/>
+      <c r="E113" s="8">
+        <v>7</v>
+      </c>
+      <c r="F113" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G113" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="H113" s="6">
         <v>9952604</v>
       </c>
@@ -4501,7 +4537,7 @@
       <c r="J113" s="9"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="8">
+      <c r="A114" s="12">
         <v>1</v>
       </c>
       <c r="B114" s="8">
@@ -4513,9 +4549,15 @@
       <c r="D114" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="E114" s="8"/>
-      <c r="F114" s="8"/>
-      <c r="G114" s="10"/>
+      <c r="E114" s="8">
+        <v>1</v>
+      </c>
+      <c r="F114" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G114" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="H114" s="6">
         <v>4407849</v>
       </c>
@@ -4523,7 +4565,7 @@
       <c r="J114" s="9"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="8">
+      <c r="A115" s="12">
         <v>1</v>
       </c>
       <c r="B115" s="8">
@@ -4535,9 +4577,15 @@
       <c r="D115" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E115" s="8"/>
-      <c r="F115" s="8"/>
-      <c r="G115" s="10"/>
+      <c r="E115" s="8">
+        <v>7</v>
+      </c>
+      <c r="F115" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G115" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="H115" s="6">
         <v>52092009</v>
       </c>
@@ -4545,7 +4593,7 @@
       <c r="J115" s="9"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="8">
+      <c r="A116" s="12">
         <v>1</v>
       </c>
       <c r="B116" s="8">
@@ -4557,9 +4605,15 @@
       <c r="D116" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="E116" s="8"/>
-      <c r="F116" s="8"/>
-      <c r="G116" s="10"/>
+      <c r="E116" s="8">
+        <v>51</v>
+      </c>
+      <c r="F116" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G116" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="H116" s="6">
         <v>669600</v>
       </c>
@@ -4567,7 +4621,7 @@
       <c r="J116" s="9"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="8">
+      <c r="A117" s="12">
         <v>1</v>
       </c>
       <c r="B117" s="8">
@@ -4579,9 +4633,15 @@
       <c r="D117" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="E117" s="8"/>
-      <c r="F117" s="8"/>
-      <c r="G117" s="10"/>
+      <c r="E117" s="8">
+        <v>7</v>
+      </c>
+      <c r="F117" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G117" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="H117" s="6">
         <v>18089916</v>
       </c>
@@ -4589,7 +4649,7 @@
       <c r="J117" s="9"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="8">
+      <c r="A118" s="12">
         <v>1</v>
       </c>
       <c r="B118" s="8">
@@ -4601,9 +4661,15 @@
       <c r="D118" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E118" s="8"/>
-      <c r="F118" s="8"/>
-      <c r="G118" s="10"/>
+      <c r="E118" s="8">
+        <v>7</v>
+      </c>
+      <c r="F118" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G118" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="H118" s="6">
         <v>4094318</v>
       </c>
@@ -4611,7 +4677,7 @@
       <c r="J118" s="9"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="8">
+      <c r="A119" s="12">
         <v>1</v>
       </c>
       <c r="B119" s="8">
@@ -4623,9 +4689,15 @@
       <c r="D119" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E119" s="8"/>
-      <c r="F119" s="8"/>
-      <c r="G119" s="10"/>
+      <c r="E119" s="8">
+        <v>7</v>
+      </c>
+      <c r="F119" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G119" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="H119" s="6">
         <v>4031339</v>
       </c>
@@ -6714,12 +6786,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002B6B606D19F8C64C9C79835747E2E002" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1490ca6afe76db67316394b374b3fffa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a52c2c93-1616-4696-bc88-4a2586572708" xmlns:ns4="44ef142f-35ce-48df-bc44-191ee5827fd0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f03ce17d5f7f795edd6d7d0ee76cdef5" ns3:_="" ns4:_="">
     <xsd:import namespace="a52c2c93-1616-4696-bc88-4a2586572708"/>
@@ -6942,6 +7008,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6952,23 +7024,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA6490E-A2D4-4F41-902E-623575711A1D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="44ef142f-35ce-48df-bc44-191ee5827fd0"/>
-    <ds:schemaRef ds:uri="a52c2c93-1616-4696-bc88-4a2586572708"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1E61E25-AEDA-4F7D-AB2D-2A0978BE05A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6987,6 +7042,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA6490E-A2D4-4F41-902E-623575711A1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="44ef142f-35ce-48df-bc44-191ee5827fd0"/>
+    <ds:schemaRef ds:uri="a52c2c93-1616-4696-bc88-4a2586572708"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4CA132-BAA9-487C-B8CA-1DC25345625A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
se soluciona version 1.1 ok
</commit_message>
<xml_diff>
--- a/PAGOPROVEEDORES.xlsx
+++ b/PAGOPROVEEDORES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Forero\Desktop\Pago-proveedores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\pago-proveedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976AA038-BA1F-4673-B902-785E3E9E0C52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42857FE-6239-47D1-8DD1-5D95D16863F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1815" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,25 +18,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$J$106</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="286">
   <si>
     <t>Tipo de Identificacion</t>
   </si>
@@ -854,115 +846,46 @@
     <t>3100000409</t>
   </si>
   <si>
+    <t>898778778</t>
+  </si>
+  <si>
+    <t>CIMAZ</t>
+  </si>
+  <si>
+    <t>S.A.S</t>
+  </si>
+  <si>
+    <t>9887987</t>
+  </si>
+  <si>
+    <t>CARINA IMPATA RESTREPO</t>
+  </si>
+  <si>
+    <t>79787</t>
+  </si>
+  <si>
+    <t>DIGITALTIC</t>
+  </si>
+  <si>
+    <t>87988797</t>
+  </si>
+  <si>
+    <t>DOMINGO</t>
+  </si>
+  <si>
+    <t>IGNACIO ROJAS</t>
+  </si>
+  <si>
+    <t>87987987</t>
+  </si>
+  <si>
     <t>BIBO</t>
   </si>
   <si>
     <t>SOLUTIONS SAS</t>
   </si>
   <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>CIMAZ</t>
-  </si>
-  <si>
-    <t>S.A.S</t>
-  </si>
-  <si>
-    <t>45654654</t>
-  </si>
-  <si>
-    <t>CIMPRE</t>
-  </si>
-  <si>
-    <t>SALUD OCUPACIONAL S.A.S.</t>
-  </si>
-  <si>
-    <t>23245654</t>
-  </si>
-  <si>
-    <t>CARINA IMPATA RESTREPO</t>
-  </si>
-  <si>
-    <t>4654654</t>
-  </si>
-  <si>
-    <t>DIGITALTIC</t>
-  </si>
-  <si>
-    <t>46545465</t>
-  </si>
-  <si>
-    <t>ELECTRICOS</t>
-  </si>
-  <si>
-    <t>DEL VALLE SA</t>
-  </si>
-  <si>
-    <t>5464654</t>
-  </si>
-  <si>
-    <t>ELECTRO</t>
-  </si>
-  <si>
-    <t>JAPONESA S.A.</t>
-  </si>
-  <si>
-    <t>GVS</t>
-  </si>
-  <si>
-    <t>COLOMBIA SAS</t>
-  </si>
-  <si>
-    <t>564654654</t>
-  </si>
-  <si>
-    <t>Hp</t>
-  </si>
-  <si>
-    <t>Financial Services Colombia LLC Sucursal Colombia</t>
-  </si>
-  <si>
-    <t>46565454</t>
-  </si>
-  <si>
-    <t>IZC</t>
-  </si>
-  <si>
-    <t>MAYORISTA SAS</t>
-  </si>
-  <si>
-    <t>4654654645</t>
-  </si>
-  <si>
-    <t>LILIUM</t>
-  </si>
-  <si>
-    <t>TECNOLOGIA SAS</t>
-  </si>
-  <si>
-    <t>98798798</t>
-  </si>
-  <si>
-    <t>NEXSYS</t>
-  </si>
-  <si>
-    <t>DE COLOMBIA SA</t>
-  </si>
-  <si>
-    <t>46564</t>
-  </si>
-  <si>
-    <t>65454654</t>
-  </si>
-  <si>
-    <t>13213213</t>
-  </si>
-  <si>
-    <t>64556654</t>
-  </si>
-  <si>
-    <t>654654654</t>
+    <t>878798778</t>
   </si>
 </sst>
 </file>
@@ -1379,10 +1302,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:J257"/>
+  <dimension ref="A1:J238"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I106" sqref="I106"/>
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4375,53 +4298,53 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B107" s="8">
-        <v>9008585507</v>
+        <v>800179308</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>272</v>
+        <v>108</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>273</v>
+        <v>36</v>
       </c>
       <c r="E107" s="8">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="F107" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H107" s="6">
-        <v>2359386</v>
+        <v>37501725</v>
       </c>
       <c r="I107" s="1"/>
       <c r="J107" s="9"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B108" s="8">
         <v>900654100</v>
       </c>
       <c r="C108" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E108" s="8">
+        <v>7</v>
+      </c>
+      <c r="F108" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G108" s="10" t="s">
         <v>275</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E108" s="8">
-        <v>51</v>
-      </c>
-      <c r="F108" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G108" s="10" t="s">
-        <v>277</v>
       </c>
       <c r="H108" s="6">
         <v>525870</v>
@@ -4434,25 +4357,25 @@
         <v>1</v>
       </c>
       <c r="B109" s="8">
-        <v>90036484392</v>
+        <v>31322510</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E109" s="8">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="F109" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H109" s="6">
-        <v>87451</v>
+        <v>84300</v>
       </c>
       <c r="I109" s="1"/>
       <c r="J109" s="9"/>
@@ -4462,25 +4385,25 @@
         <v>3</v>
       </c>
       <c r="B110" s="8">
-        <v>31322510</v>
+        <v>901223156</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>241</v>
+        <v>278</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>281</v>
+        <v>36</v>
       </c>
       <c r="E110" s="8">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="F110" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G110" s="10" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H110" s="6">
-        <v>84300</v>
+        <v>193970</v>
       </c>
       <c r="I110" s="1"/>
       <c r="J110" s="9"/>
@@ -4490,13 +4413,13 @@
         <v>1</v>
       </c>
       <c r="B111" s="8">
-        <v>9012231566</v>
+        <v>72156499</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>36</v>
+        <v>281</v>
       </c>
       <c r="E111" s="8">
         <v>7</v>
@@ -4505,26 +4428,26 @@
         <v>12</v>
       </c>
       <c r="G111" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H111" s="6">
-        <v>193970</v>
+        <v>97991</v>
       </c>
       <c r="I111" s="1"/>
       <c r="J111" s="9"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B112" s="8">
-        <v>8903043450</v>
+        <v>9008585507</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E112" s="8">
         <v>7</v>
@@ -4533,291 +4456,131 @@
         <v>12</v>
       </c>
       <c r="G112" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H112" s="6">
-        <v>172500</v>
+        <v>2359386</v>
       </c>
       <c r="I112" s="1"/>
       <c r="J112" s="9"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="8">
-        <v>1</v>
-      </c>
-      <c r="B113" s="8">
-        <v>890306372</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E113" s="8">
-        <v>51</v>
-      </c>
-      <c r="F113" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G113" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="H113" s="6">
-        <v>1819546</v>
-      </c>
+      <c r="A113" s="8"/>
+      <c r="B113" s="8"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="8"/>
+      <c r="F113" s="8"/>
+      <c r="G113" s="10"/>
+      <c r="H113" s="6"/>
       <c r="I113" s="1"/>
       <c r="J113" s="9"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="8">
-        <v>1</v>
-      </c>
-      <c r="B114" s="8">
-        <v>9002980749</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="E114" s="8">
-        <v>7</v>
-      </c>
-      <c r="F114" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G114" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="H114" s="6">
-        <v>9952604</v>
-      </c>
+      <c r="A114" s="8"/>
+      <c r="B114" s="8"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="8"/>
+      <c r="F114" s="8"/>
+      <c r="G114" s="10"/>
+      <c r="H114" s="6"/>
       <c r="I114" s="1"/>
       <c r="J114" s="9"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="8">
-        <v>1</v>
-      </c>
-      <c r="B115" s="8">
-        <v>830076882</v>
-      </c>
-      <c r="C115" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E115" s="8">
-        <v>51</v>
-      </c>
-      <c r="F115" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G115" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="H115" s="6">
-        <v>4407849</v>
-      </c>
+      <c r="A115" s="8"/>
+      <c r="B115" s="8"/>
+      <c r="C115" s="8"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="8"/>
+      <c r="F115" s="8"/>
+      <c r="G115" s="10"/>
+      <c r="H115" s="6"/>
       <c r="I115" s="1"/>
       <c r="J115" s="9"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="8">
-        <v>1</v>
-      </c>
-      <c r="B116" s="8">
-        <v>11439407226</v>
-      </c>
-      <c r="C116" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="E116" s="8">
-        <v>7</v>
-      </c>
-      <c r="F116" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G116" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="H116" s="6">
-        <v>52092009</v>
-      </c>
+      <c r="A116" s="8"/>
+      <c r="B116" s="8"/>
+      <c r="C116" s="8"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="8"/>
+      <c r="F116" s="8"/>
+      <c r="G116" s="10"/>
+      <c r="H116" s="6"/>
       <c r="I116" s="1"/>
       <c r="J116" s="9"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="8">
-        <v>1</v>
-      </c>
-      <c r="B117" s="8">
-        <v>9008928419</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E117" s="8">
-        <v>7</v>
-      </c>
-      <c r="F117" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G117" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="H117" s="6">
-        <v>669600</v>
-      </c>
+      <c r="A117" s="8"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="8"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="8"/>
+      <c r="F117" s="8"/>
+      <c r="G117" s="10"/>
+      <c r="H117" s="6"/>
       <c r="I117" s="1"/>
       <c r="J117" s="9"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="8">
-        <v>1</v>
-      </c>
-      <c r="B118" s="8">
-        <v>800035776</v>
-      </c>
-      <c r="C118" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="E118" s="8">
-        <v>51</v>
-      </c>
-      <c r="F118" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G118" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="H118" s="6">
-        <v>18089916</v>
-      </c>
+      <c r="A118" s="8"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="8"/>
+      <c r="F118" s="8"/>
+      <c r="G118" s="10"/>
+      <c r="H118" s="6"/>
       <c r="I118" s="1"/>
       <c r="J118" s="9"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="8">
-        <v>1</v>
-      </c>
-      <c r="B119" s="8">
-        <v>8300343439</v>
-      </c>
-      <c r="C119" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E119" s="8">
-        <v>7</v>
-      </c>
-      <c r="F119" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G119" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="H119" s="6">
-        <v>4094318</v>
-      </c>
+      <c r="A119" s="8"/>
+      <c r="B119" s="8"/>
+      <c r="C119" s="8"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="8"/>
+      <c r="F119" s="8"/>
+      <c r="G119" s="10"/>
+      <c r="H119" s="6"/>
       <c r="I119" s="1"/>
       <c r="J119" s="9"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="8">
-        <v>1</v>
-      </c>
-      <c r="B120" s="8">
-        <v>8001793084</v>
-      </c>
-      <c r="C120" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E120" s="8">
-        <v>7</v>
-      </c>
-      <c r="F120" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G120" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="H120" s="6">
-        <v>4031339</v>
-      </c>
+      <c r="A120" s="8"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="1"/>
+      <c r="E120" s="8"/>
+      <c r="F120" s="8"/>
+      <c r="G120" s="10"/>
+      <c r="H120" s="6"/>
       <c r="I120" s="1"/>
       <c r="J120" s="9"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" s="8">
-        <v>1</v>
-      </c>
-      <c r="B121" s="8">
-        <v>9008585507</v>
-      </c>
-      <c r="C121" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E121" s="8">
-        <v>7</v>
-      </c>
-      <c r="F121" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G121" s="10" t="s">
-        <v>307</v>
-      </c>
-      <c r="H121" s="6">
-        <v>2359386</v>
-      </c>
+      <c r="A121" s="8"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="8"/>
+      <c r="D121" s="1"/>
+      <c r="E121" s="8"/>
+      <c r="F121" s="8"/>
+      <c r="G121" s="10"/>
+      <c r="H121" s="6"/>
       <c r="I121" s="1"/>
       <c r="J121" s="9"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" s="8">
-        <v>1</v>
-      </c>
-      <c r="B122" s="8">
-        <v>800179308</v>
-      </c>
-      <c r="C122" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E122" s="8">
-        <v>51</v>
-      </c>
-      <c r="F122" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G122" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="H122" s="6">
-        <v>37501725</v>
-      </c>
+      <c r="A122" s="8"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="8"/>
+      <c r="F122" s="8"/>
+      <c r="G122" s="10"/>
+      <c r="H122" s="6"/>
       <c r="I122" s="1"/>
       <c r="J122" s="9"/>
     </row>
@@ -6212,234 +5975,6 @@
       <c r="H238" s="6"/>
       <c r="I238" s="1"/>
       <c r="J238" s="9"/>
-    </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A239" s="8"/>
-      <c r="B239" s="8"/>
-      <c r="C239" s="8"/>
-      <c r="D239" s="1"/>
-      <c r="E239" s="8"/>
-      <c r="F239" s="8"/>
-      <c r="G239" s="10"/>
-      <c r="H239" s="6"/>
-      <c r="I239" s="1"/>
-      <c r="J239" s="9"/>
-    </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A240" s="8"/>
-      <c r="B240" s="8"/>
-      <c r="C240" s="8"/>
-      <c r="D240" s="1"/>
-      <c r="E240" s="8"/>
-      <c r="F240" s="8"/>
-      <c r="G240" s="10"/>
-      <c r="H240" s="6"/>
-      <c r="I240" s="1"/>
-      <c r="J240" s="9"/>
-    </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A241" s="8"/>
-      <c r="B241" s="8"/>
-      <c r="C241" s="8"/>
-      <c r="D241" s="1"/>
-      <c r="E241" s="8"/>
-      <c r="F241" s="8"/>
-      <c r="G241" s="10"/>
-      <c r="H241" s="6"/>
-      <c r="I241" s="1"/>
-      <c r="J241" s="9"/>
-    </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A242" s="8"/>
-      <c r="B242" s="8"/>
-      <c r="C242" s="8"/>
-      <c r="D242" s="1"/>
-      <c r="E242" s="8"/>
-      <c r="F242" s="8"/>
-      <c r="G242" s="10"/>
-      <c r="H242" s="6"/>
-      <c r="I242" s="1"/>
-      <c r="J242" s="9"/>
-    </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A243" s="8"/>
-      <c r="B243" s="8"/>
-      <c r="C243" s="8"/>
-      <c r="D243" s="1"/>
-      <c r="E243" s="8"/>
-      <c r="F243" s="8"/>
-      <c r="G243" s="10"/>
-      <c r="H243" s="6"/>
-      <c r="I243" s="1"/>
-      <c r="J243" s="9"/>
-    </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A244" s="8"/>
-      <c r="B244" s="8"/>
-      <c r="C244" s="8"/>
-      <c r="D244" s="1"/>
-      <c r="E244" s="8"/>
-      <c r="F244" s="8"/>
-      <c r="G244" s="10"/>
-      <c r="H244" s="6"/>
-      <c r="I244" s="1"/>
-      <c r="J244" s="9"/>
-    </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A245" s="8"/>
-      <c r="B245" s="8"/>
-      <c r="C245" s="8"/>
-      <c r="D245" s="1"/>
-      <c r="E245" s="8"/>
-      <c r="F245" s="8"/>
-      <c r="G245" s="10"/>
-      <c r="H245" s="6"/>
-      <c r="I245" s="1"/>
-      <c r="J245" s="9"/>
-    </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A246" s="8"/>
-      <c r="B246" s="8"/>
-      <c r="C246" s="8"/>
-      <c r="D246" s="1"/>
-      <c r="E246" s="8"/>
-      <c r="F246" s="8"/>
-      <c r="G246" s="10"/>
-      <c r="H246" s="6"/>
-      <c r="I246" s="1"/>
-      <c r="J246" s="9"/>
-    </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A247" s="8"/>
-      <c r="B247" s="8"/>
-      <c r="C247" s="8"/>
-      <c r="D247" s="1"/>
-      <c r="E247" s="8"/>
-      <c r="F247" s="8"/>
-      <c r="G247" s="10"/>
-      <c r="H247" s="6"/>
-      <c r="I247" s="1"/>
-      <c r="J247" s="9"/>
-    </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A248" s="8"/>
-      <c r="B248" s="8"/>
-      <c r="C248" s="8"/>
-      <c r="D248" s="1"/>
-      <c r="E248" s="8"/>
-      <c r="F248" s="8"/>
-      <c r="G248" s="10"/>
-      <c r="H248" s="6"/>
-      <c r="I248" s="1"/>
-      <c r="J248" s="9"/>
-    </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A249" s="8"/>
-      <c r="B249" s="8"/>
-      <c r="C249" s="8"/>
-      <c r="D249" s="1"/>
-      <c r="E249" s="8"/>
-      <c r="F249" s="8"/>
-      <c r="G249" s="10"/>
-      <c r="H249" s="6"/>
-      <c r="I249" s="1"/>
-      <c r="J249" s="9"/>
-    </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A250" s="8"/>
-      <c r="B250" s="8"/>
-      <c r="C250" s="8"/>
-      <c r="D250" s="1"/>
-      <c r="E250" s="8"/>
-      <c r="F250" s="8"/>
-      <c r="G250" s="10"/>
-      <c r="H250" s="6"/>
-      <c r="I250" s="1"/>
-      <c r="J250" s="9"/>
-    </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A251" s="8"/>
-      <c r="B251" s="8"/>
-      <c r="C251" s="8"/>
-      <c r="D251" s="1"/>
-      <c r="E251" s="8"/>
-      <c r="F251" s="8"/>
-      <c r="G251" s="10"/>
-      <c r="H251" s="6"/>
-      <c r="I251" s="1"/>
-      <c r="J251" s="9"/>
-    </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A252" s="8"/>
-      <c r="B252" s="8"/>
-      <c r="C252" s="8"/>
-      <c r="D252" s="1"/>
-      <c r="E252" s="8"/>
-      <c r="F252" s="8"/>
-      <c r="G252" s="10"/>
-      <c r="H252" s="6"/>
-      <c r="I252" s="1"/>
-      <c r="J252" s="9"/>
-    </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A253" s="8"/>
-      <c r="B253" s="8"/>
-      <c r="C253" s="8"/>
-      <c r="D253" s="1"/>
-      <c r="E253" s="8"/>
-      <c r="F253" s="8"/>
-      <c r="G253" s="10"/>
-      <c r="H253" s="6"/>
-      <c r="I253" s="1"/>
-      <c r="J253" s="9"/>
-    </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A254" s="8"/>
-      <c r="B254" s="8"/>
-      <c r="C254" s="8"/>
-      <c r="D254" s="1"/>
-      <c r="E254" s="8"/>
-      <c r="F254" s="8"/>
-      <c r="G254" s="10"/>
-      <c r="H254" s="6"/>
-      <c r="I254" s="1"/>
-      <c r="J254" s="9"/>
-    </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A255" s="8"/>
-      <c r="B255" s="8"/>
-      <c r="C255" s="8"/>
-      <c r="D255" s="1"/>
-      <c r="E255" s="8"/>
-      <c r="F255" s="8"/>
-      <c r="G255" s="10"/>
-      <c r="H255" s="6"/>
-      <c r="I255" s="1"/>
-      <c r="J255" s="9"/>
-    </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A256" s="8"/>
-      <c r="B256" s="8"/>
-      <c r="C256" s="8"/>
-      <c r="D256" s="1"/>
-      <c r="E256" s="8"/>
-      <c r="F256" s="8"/>
-      <c r="G256" s="10"/>
-      <c r="H256" s="6"/>
-      <c r="I256" s="1"/>
-      <c r="J256" s="9"/>
-    </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A257" s="8"/>
-      <c r="B257" s="8"/>
-      <c r="C257" s="8"/>
-      <c r="D257" s="1"/>
-      <c r="E257" s="8"/>
-      <c r="F257" s="8"/>
-      <c r="G257" s="10"/>
-      <c r="H257" s="6"/>
-      <c r="I257" s="1"/>
-      <c r="J257" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J106" xr:uid="{362F9B73-73C4-443B-849C-D7B08CE211DA}"/>
@@ -6460,12 +5995,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6474,7 +6003,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002B6B606D19F8C64C9C79835747E2E002" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1490ca6afe76db67316394b374b3fffa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a52c2c93-1616-4696-bc88-4a2586572708" xmlns:ns4="44ef142f-35ce-48df-bc44-191ee5827fd0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f03ce17d5f7f795edd6d7d0ee76cdef5" ns3:_="" ns4:_="">
     <xsd:import namespace="a52c2c93-1616-4696-bc88-4a2586572708"/>
@@ -6697,24 +6226,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA6490E-A2D4-4F41-902E-623575711A1D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="44ef142f-35ce-48df-bc44-191ee5827fd0"/>
-    <ds:schemaRef ds:uri="a52c2c93-1616-4696-bc88-4a2586572708"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4CA132-BAA9-487C-B8CA-1DC25345625A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -6722,7 +6240,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1E61E25-AEDA-4F7D-AB2D-2A0978BE05A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6739,4 +6257,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA6490E-A2D4-4F41-902E-623575711A1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="44ef142f-35ce-48df-bc44-191ee5827fd0"/>
+    <ds:schemaRef ds:uri="a52c2c93-1616-4696-bc88-4a2586572708"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
se agrega hora para guradar archivo de bancos
</commit_message>
<xml_diff>
--- a/PAGOPROVEEDORES.xlsx
+++ b/PAGOPROVEEDORES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\pago-proveedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42857FE-6239-47D1-8DD1-5D95D16863F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557AC0BD-4710-4FF1-88F5-F25A254D6A44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="280">
   <si>
     <t>Tipo de Identificacion</t>
   </si>
@@ -846,46 +846,28 @@
     <t>3100000409</t>
   </si>
   <si>
-    <t>898778778</t>
-  </si>
-  <si>
     <t>CIMAZ</t>
   </si>
   <si>
     <t>S.A.S</t>
   </si>
   <si>
-    <t>9887987</t>
-  </si>
-  <si>
     <t>CARINA IMPATA RESTREPO</t>
   </si>
   <si>
-    <t>79787</t>
-  </si>
-  <si>
-    <t>DIGITALTIC</t>
-  </si>
-  <si>
-    <t>87988797</t>
-  </si>
-  <si>
-    <t>DOMINGO</t>
-  </si>
-  <si>
-    <t>IGNACIO ROJAS</t>
-  </si>
-  <si>
-    <t>87987987</t>
-  </si>
-  <si>
     <t>BIBO</t>
   </si>
   <si>
     <t>SOLUTIONS SAS</t>
   </si>
   <si>
-    <t>878798778</t>
+    <t>898098</t>
+  </si>
+  <si>
+    <t>8098098</t>
+  </si>
+  <si>
+    <t>87897987</t>
   </si>
 </sst>
 </file>
@@ -1302,10 +1284,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:J238"/>
+  <dimension ref="A1:J231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4301,13 +4283,13 @@
         <v>3</v>
       </c>
       <c r="B107" s="8">
-        <v>800179308</v>
+        <v>9008585507</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>108</v>
+        <v>275</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>36</v>
+        <v>276</v>
       </c>
       <c r="E107" s="8">
         <v>51</v>
@@ -4316,10 +4298,10 @@
         <v>10</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="H107" s="6">
-        <v>37501725</v>
+        <v>2359386</v>
       </c>
       <c r="I107" s="1"/>
       <c r="J107" s="9"/>
@@ -4332,10 +4314,10 @@
         <v>900654100</v>
       </c>
       <c r="C108" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="E108" s="8">
         <v>7</v>
@@ -4344,7 +4326,7 @@
         <v>12</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H108" s="6">
         <v>525870</v>
@@ -4363,16 +4345,16 @@
         <v>241</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E109" s="8">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="F109" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="H109" s="6">
         <v>84300</v>
@@ -4381,86 +4363,38 @@
       <c r="J109" s="9"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="8">
-        <v>3</v>
-      </c>
-      <c r="B110" s="8">
-        <v>901223156</v>
-      </c>
-      <c r="C110" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E110" s="8">
-        <v>51</v>
-      </c>
-      <c r="F110" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G110" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="H110" s="6">
-        <v>193970</v>
-      </c>
+      <c r="A110" s="8"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="8"/>
+      <c r="G110" s="10"/>
+      <c r="H110" s="6"/>
       <c r="I110" s="1"/>
       <c r="J110" s="9"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="8">
-        <v>1</v>
-      </c>
-      <c r="B111" s="8">
-        <v>72156499</v>
-      </c>
-      <c r="C111" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E111" s="8">
-        <v>7</v>
-      </c>
-      <c r="F111" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G111" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="H111" s="6">
-        <v>97991</v>
-      </c>
+      <c r="A111" s="8"/>
+      <c r="B111" s="8"/>
+      <c r="C111" s="8"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="8"/>
+      <c r="F111" s="8"/>
+      <c r="G111" s="10"/>
+      <c r="H111" s="6"/>
       <c r="I111" s="1"/>
       <c r="J111" s="9"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="8">
-        <v>3</v>
-      </c>
-      <c r="B112" s="8">
-        <v>9008585507</v>
-      </c>
-      <c r="C112" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E112" s="8">
-        <v>7</v>
-      </c>
-      <c r="F112" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G112" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="H112" s="6">
-        <v>2359386</v>
-      </c>
+      <c r="A112" s="8"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="8"/>
+      <c r="F112" s="8"/>
+      <c r="G112" s="10"/>
+      <c r="H112" s="6"/>
       <c r="I112" s="1"/>
       <c r="J112" s="9"/>
     </row>
@@ -5891,90 +5825,6 @@
       <c r="H231" s="6"/>
       <c r="I231" s="1"/>
       <c r="J231" s="9"/>
-    </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A232" s="8"/>
-      <c r="B232" s="8"/>
-      <c r="C232" s="8"/>
-      <c r="D232" s="1"/>
-      <c r="E232" s="8"/>
-      <c r="F232" s="8"/>
-      <c r="G232" s="10"/>
-      <c r="H232" s="6"/>
-      <c r="I232" s="1"/>
-      <c r="J232" s="9"/>
-    </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A233" s="8"/>
-      <c r="B233" s="8"/>
-      <c r="C233" s="8"/>
-      <c r="D233" s="1"/>
-      <c r="E233" s="8"/>
-      <c r="F233" s="8"/>
-      <c r="G233" s="10"/>
-      <c r="H233" s="6"/>
-      <c r="I233" s="1"/>
-      <c r="J233" s="9"/>
-    </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A234" s="8"/>
-      <c r="B234" s="8"/>
-      <c r="C234" s="8"/>
-      <c r="D234" s="1"/>
-      <c r="E234" s="8"/>
-      <c r="F234" s="8"/>
-      <c r="G234" s="10"/>
-      <c r="H234" s="6"/>
-      <c r="I234" s="1"/>
-      <c r="J234" s="9"/>
-    </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A235" s="8"/>
-      <c r="B235" s="8"/>
-      <c r="C235" s="8"/>
-      <c r="D235" s="1"/>
-      <c r="E235" s="8"/>
-      <c r="F235" s="8"/>
-      <c r="G235" s="10"/>
-      <c r="H235" s="6"/>
-      <c r="I235" s="1"/>
-      <c r="J235" s="9"/>
-    </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A236" s="8"/>
-      <c r="B236" s="8"/>
-      <c r="C236" s="8"/>
-      <c r="D236" s="1"/>
-      <c r="E236" s="8"/>
-      <c r="F236" s="8"/>
-      <c r="G236" s="10"/>
-      <c r="H236" s="6"/>
-      <c r="I236" s="1"/>
-      <c r="J236" s="9"/>
-    </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A237" s="8"/>
-      <c r="B237" s="8"/>
-      <c r="C237" s="8"/>
-      <c r="D237" s="1"/>
-      <c r="E237" s="8"/>
-      <c r="F237" s="8"/>
-      <c r="G237" s="10"/>
-      <c r="H237" s="6"/>
-      <c r="I237" s="1"/>
-      <c r="J237" s="9"/>
-    </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A238" s="8"/>
-      <c r="B238" s="8"/>
-      <c r="C238" s="8"/>
-      <c r="D238" s="1"/>
-      <c r="E238" s="8"/>
-      <c r="F238" s="8"/>
-      <c r="G238" s="10"/>
-      <c r="H238" s="6"/>
-      <c r="I238" s="1"/>
-      <c r="J238" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J106" xr:uid="{362F9B73-73C4-443B-849C-D7B08CE211DA}"/>
@@ -5995,6 +5845,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6003,7 +5859,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002B6B606D19F8C64C9C79835747E2E002" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1490ca6afe76db67316394b374b3fffa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a52c2c93-1616-4696-bc88-4a2586572708" xmlns:ns4="44ef142f-35ce-48df-bc44-191ee5827fd0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f03ce17d5f7f795edd6d7d0ee76cdef5" ns3:_="" ns4:_="">
     <xsd:import namespace="a52c2c93-1616-4696-bc88-4a2586572708"/>
@@ -6226,13 +6082,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA6490E-A2D4-4F41-902E-623575711A1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="44ef142f-35ce-48df-bc44-191ee5827fd0"/>
+    <ds:schemaRef ds:uri="a52c2c93-1616-4696-bc88-4a2586572708"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4CA132-BAA9-487C-B8CA-1DC25345625A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -6240,7 +6107,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1E61E25-AEDA-4F7D-AB2D-2A0978BE05A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6257,21 +6124,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA6490E-A2D4-4F41-902E-623575711A1D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="44ef142f-35ce-48df-bc44-191ee5827fd0"/>
-    <ds:schemaRef ds:uri="a52c2c93-1616-4696-bc88-4a2586572708"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
version 1.2 validacion A2, B2 en hoja Datos; ok
</commit_message>
<xml_diff>
--- a/PAGOPROVEEDORES.xlsx
+++ b/PAGOPROVEEDORES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\pago-proveedores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Forero\Desktop\Pago-proveedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB899C83-72BD-45F0-8BBB-B26852A06C56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9477D5F7-794A-4F39-B73A-651E01027B08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,17 +18,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$J$106</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="281">
   <si>
     <t>Tipo de Identificacion</t>
   </si>
@@ -852,22 +860,25 @@
     <t>S.A.S</t>
   </si>
   <si>
+    <t>4654654645</t>
+  </si>
+  <si>
+    <t>546564</t>
+  </si>
+  <si>
     <t>CARINA IMPATA RESTREPO</t>
   </si>
   <si>
-    <t>BIBO</t>
-  </si>
-  <si>
-    <t>SOLUTIONS SAS</t>
-  </si>
-  <si>
-    <t>898098</t>
-  </si>
-  <si>
-    <t>8098098</t>
-  </si>
-  <si>
-    <t>87897987</t>
+    <t>656456654</t>
+  </si>
+  <si>
+    <t>DIGITALTIC</t>
+  </si>
+  <si>
+    <t>45465465</t>
+  </si>
+  <si>
+    <t>BIBO SOLUTIONS SAS</t>
   </si>
 </sst>
 </file>
@@ -1284,10 +1295,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:J231"/>
+  <dimension ref="A1:J227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4286,19 +4297,19 @@
         <v>9008585507</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E107" s="8">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="F107" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H107" s="6">
         <v>2359386</v>
@@ -4311,7 +4322,7 @@
         <v>3</v>
       </c>
       <c r="B108" s="8">
-        <v>900654100</v>
+        <v>9006541001</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>272</v>
@@ -4326,7 +4337,7 @@
         <v>12</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H108" s="6">
         <v>525870</v>
@@ -4345,16 +4356,16 @@
         <v>241</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="E109" s="8">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H109" s="6">
         <v>84300</v>
@@ -4367,19 +4378,25 @@
         <v>3</v>
       </c>
       <c r="B110" s="8">
-        <v>9006541001</v>
+        <v>901223156</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E110" s="8"/>
-      <c r="F110" s="8"/>
-      <c r="G110" s="10"/>
+        <v>36</v>
+      </c>
+      <c r="E110" s="8">
+        <v>51</v>
+      </c>
+      <c r="F110" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G110" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="H110" s="6">
-        <v>2359386</v>
+        <v>193970</v>
       </c>
       <c r="I110" s="1"/>
       <c r="J110" s="9"/>
@@ -5787,54 +5804,6 @@
       <c r="H227" s="6"/>
       <c r="I227" s="1"/>
       <c r="J227" s="9"/>
-    </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A228" s="8"/>
-      <c r="B228" s="8"/>
-      <c r="C228" s="8"/>
-      <c r="D228" s="1"/>
-      <c r="E228" s="8"/>
-      <c r="F228" s="8"/>
-      <c r="G228" s="10"/>
-      <c r="H228" s="6"/>
-      <c r="I228" s="1"/>
-      <c r="J228" s="9"/>
-    </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A229" s="8"/>
-      <c r="B229" s="8"/>
-      <c r="C229" s="8"/>
-      <c r="D229" s="1"/>
-      <c r="E229" s="8"/>
-      <c r="F229" s="8"/>
-      <c r="G229" s="10"/>
-      <c r="H229" s="6"/>
-      <c r="I229" s="1"/>
-      <c r="J229" s="9"/>
-    </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A230" s="8"/>
-      <c r="B230" s="8"/>
-      <c r="C230" s="8"/>
-      <c r="D230" s="1"/>
-      <c r="E230" s="8"/>
-      <c r="F230" s="8"/>
-      <c r="G230" s="10"/>
-      <c r="H230" s="6"/>
-      <c r="I230" s="1"/>
-      <c r="J230" s="9"/>
-    </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A231" s="8"/>
-      <c r="B231" s="8"/>
-      <c r="C231" s="8"/>
-      <c r="D231" s="1"/>
-      <c r="E231" s="8"/>
-      <c r="F231" s="8"/>
-      <c r="G231" s="10"/>
-      <c r="H231" s="6"/>
-      <c r="I231" s="1"/>
-      <c r="J231" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J106" xr:uid="{362F9B73-73C4-443B-849C-D7B08CE211DA}"/>
@@ -5855,15 +5824,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002B6B606D19F8C64C9C79835747E2E002" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1490ca6afe76db67316394b374b3fffa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a52c2c93-1616-4696-bc88-4a2586572708" xmlns:ns4="44ef142f-35ce-48df-bc44-191ee5827fd0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f03ce17d5f7f795edd6d7d0ee76cdef5" ns3:_="" ns4:_="">
     <xsd:import namespace="a52c2c93-1616-4696-bc88-4a2586572708"/>
@@ -6086,6 +6046,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -6093,14 +6062,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4CA132-BAA9-487C-B8CA-1DC25345625A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1E61E25-AEDA-4F7D-AB2D-2A0978BE05A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6115,6 +6076,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4CA132-BAA9-487C-B8CA-1DC25345625A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Se finaliza documentacion y pruebas version 1.2
</commit_message>
<xml_diff>
--- a/PAGOPROVEEDORES.xlsx
+++ b/PAGOPROVEEDORES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Forero\Desktop\Pago-proveedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254AF01E-FFB7-4002-9960-C39647BB6838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759F3833-8530-4726-8E07-E9411ECF3D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1815" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="303">
   <si>
     <t>Tipo de Identificacion</t>
   </si>
@@ -879,6 +879,72 @@
   </si>
   <si>
     <t>BIBO SOLUTIONS SAS</t>
+  </si>
+  <si>
+    <t>CIMPRE</t>
+  </si>
+  <si>
+    <t>SALUD OCUPACIONAL S.A.S.</t>
+  </si>
+  <si>
+    <t>ELECTRICOS</t>
+  </si>
+  <si>
+    <t>DEL VALLE SA</t>
+  </si>
+  <si>
+    <t>4565465465</t>
+  </si>
+  <si>
+    <t>Hp</t>
+  </si>
+  <si>
+    <t>Financial Services Colombia LLC Sucursal Colombia</t>
+  </si>
+  <si>
+    <t>4654654</t>
+  </si>
+  <si>
+    <t>IZC</t>
+  </si>
+  <si>
+    <t>MAYORISTA SAS</t>
+  </si>
+  <si>
+    <t>4565654</t>
+  </si>
+  <si>
+    <t>LILIUM</t>
+  </si>
+  <si>
+    <t>TECNOLOGIA SAS</t>
+  </si>
+  <si>
+    <t>465654</t>
+  </si>
+  <si>
+    <t>NEXSYS</t>
+  </si>
+  <si>
+    <t>DE COLOMBIA SA</t>
+  </si>
+  <si>
+    <t>6546546</t>
+  </si>
+  <si>
+    <t>465464</t>
+  </si>
+  <si>
+    <t>65464</t>
+  </si>
+  <si>
+    <t>6465454456</t>
+  </si>
+  <si>
+    <t>45656465</t>
+  </si>
+  <si>
+    <t>46565464</t>
   </si>
 </sst>
 </file>
@@ -1297,8 +1363,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:J227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F108" sqref="F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4402,122 +4468,282 @@
       <c r="J110" s="9"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="8"/>
-      <c r="B111" s="8"/>
-      <c r="C111" s="8"/>
-      <c r="D111" s="1"/>
-      <c r="E111" s="8"/>
-      <c r="F111" s="8"/>
-      <c r="G111" s="10"/>
-      <c r="H111" s="6"/>
+      <c r="A111" s="8">
+        <v>3</v>
+      </c>
+      <c r="B111" s="8">
+        <v>90036484392</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E111" s="8">
+        <v>51</v>
+      </c>
+      <c r="F111" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G111" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="H111" s="6">
+        <v>87451</v>
+      </c>
       <c r="I111" s="1"/>
       <c r="J111" s="9"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="8"/>
-      <c r="B112" s="8"/>
-      <c r="C112" s="8"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="8"/>
-      <c r="G112" s="10"/>
-      <c r="H112" s="6"/>
+      <c r="A112" s="8">
+        <v>3</v>
+      </c>
+      <c r="B112" s="8">
+        <v>8903043450</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E112" s="8">
+        <v>51</v>
+      </c>
+      <c r="F112" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G112" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="H112" s="6">
+        <v>172500</v>
+      </c>
       <c r="I112" s="1"/>
       <c r="J112" s="9"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="8"/>
-      <c r="B113" s="8"/>
-      <c r="C113" s="8"/>
-      <c r="D113" s="1"/>
-      <c r="E113" s="8"/>
-      <c r="F113" s="8"/>
-      <c r="G113" s="10"/>
-      <c r="H113" s="6"/>
+      <c r="A113" s="8">
+        <v>3</v>
+      </c>
+      <c r="B113" s="8">
+        <v>830076882</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E113" s="8">
+        <v>7</v>
+      </c>
+      <c r="F113" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G113" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="H113" s="6">
+        <v>4407849</v>
+      </c>
       <c r="I113" s="1"/>
       <c r="J113" s="9"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="8"/>
-      <c r="B114" s="8"/>
-      <c r="C114" s="8"/>
-      <c r="D114" s="1"/>
-      <c r="E114" s="8"/>
-      <c r="F114" s="8"/>
-      <c r="G114" s="10"/>
-      <c r="H114" s="6"/>
+      <c r="A114" s="8">
+        <v>3</v>
+      </c>
+      <c r="B114" s="8">
+        <v>1143940722</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E114" s="8">
+        <v>7</v>
+      </c>
+      <c r="F114" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G114" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="H114" s="6">
+        <v>52092009</v>
+      </c>
       <c r="I114" s="1"/>
       <c r="J114" s="9"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="8"/>
-      <c r="B115" s="8"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="8"/>
-      <c r="F115" s="8"/>
-      <c r="G115" s="10"/>
-      <c r="H115" s="6"/>
+      <c r="A115" s="8">
+        <v>3</v>
+      </c>
+      <c r="B115" s="8">
+        <v>900892841</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E115" s="8">
+        <v>7</v>
+      </c>
+      <c r="F115" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G115" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="H115" s="6">
+        <v>669600</v>
+      </c>
       <c r="I115" s="1"/>
       <c r="J115" s="9"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="8"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="8"/>
-      <c r="D116" s="1"/>
-      <c r="E116" s="8"/>
-      <c r="F116" s="8"/>
-      <c r="G116" s="10"/>
-      <c r="H116" s="6"/>
+      <c r="A116" s="8">
+        <v>3</v>
+      </c>
+      <c r="B116" s="8">
+        <v>800035776</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E116" s="8">
+        <v>7</v>
+      </c>
+      <c r="F116" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G116" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="H116" s="6">
+        <v>18089916</v>
+      </c>
       <c r="I116" s="1"/>
       <c r="J116" s="9"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="8"/>
-      <c r="B117" s="8"/>
-      <c r="C117" s="8"/>
-      <c r="D117" s="1"/>
-      <c r="E117" s="8"/>
-      <c r="F117" s="8"/>
-      <c r="G117" s="10"/>
-      <c r="H117" s="6"/>
+      <c r="A117" s="8">
+        <v>3</v>
+      </c>
+      <c r="B117" s="8">
+        <v>830034343</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E117" s="8">
+        <v>7</v>
+      </c>
+      <c r="F117" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G117" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="H117" s="6">
+        <v>4094318</v>
+      </c>
       <c r="I117" s="1"/>
       <c r="J117" s="9"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="8"/>
-      <c r="B118" s="8"/>
-      <c r="C118" s="8"/>
-      <c r="D118" s="1"/>
-      <c r="E118" s="8"/>
-      <c r="F118" s="8"/>
-      <c r="G118" s="10"/>
-      <c r="H118" s="6"/>
+      <c r="A118" s="8">
+        <v>3</v>
+      </c>
+      <c r="B118" s="8">
+        <v>800179308</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E118" s="8">
+        <v>7</v>
+      </c>
+      <c r="F118" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G118" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="H118" s="6">
+        <v>4031339</v>
+      </c>
       <c r="I118" s="1"/>
       <c r="J118" s="9"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="8"/>
-      <c r="B119" s="8"/>
-      <c r="C119" s="8"/>
-      <c r="D119" s="1"/>
-      <c r="E119" s="8"/>
-      <c r="F119" s="8"/>
-      <c r="G119" s="10"/>
-      <c r="H119" s="6"/>
+      <c r="A119" s="8">
+        <v>3</v>
+      </c>
+      <c r="B119" s="8">
+        <v>444441</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E119" s="8">
+        <v>7</v>
+      </c>
+      <c r="F119" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G119" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="H119" s="6">
+        <v>525870</v>
+      </c>
       <c r="I119" s="1"/>
       <c r="J119" s="9"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="8"/>
-      <c r="B120" s="8"/>
-      <c r="C120" s="8"/>
-      <c r="D120" s="1"/>
-      <c r="E120" s="8"/>
-      <c r="F120" s="8"/>
-      <c r="G120" s="10"/>
-      <c r="H120" s="6"/>
+      <c r="A120" s="8">
+        <v>3</v>
+      </c>
+      <c r="B120" s="8">
+        <v>4566546546</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E120" s="8">
+        <v>51</v>
+      </c>
+      <c r="F120" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G120" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="H120" s="6">
+        <v>193970</v>
+      </c>
       <c r="I120" s="1"/>
       <c r="J120" s="9"/>
     </row>
@@ -5833,6 +6059,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002B6B606D19F8C64C9C79835747E2E002" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1490ca6afe76db67316394b374b3fffa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a52c2c93-1616-4696-bc88-4a2586572708" xmlns:ns4="44ef142f-35ce-48df-bc44-191ee5827fd0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f03ce17d5f7f795edd6d7d0ee76cdef5" ns3:_="" ns4:_="">
     <xsd:import namespace="a52c2c93-1616-4696-bc88-4a2586572708"/>
@@ -6055,12 +6287,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4CA132-BAA9-487C-B8CA-1DC25345625A}">
   <ds:schemaRefs>
@@ -6070,6 +6296,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA6490E-A2D4-4F41-902E-623575711A1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="44ef142f-35ce-48df-bc44-191ee5827fd0"/>
+    <ds:schemaRef ds:uri="a52c2c93-1616-4696-bc88-4a2586572708"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1E61E25-AEDA-4F7D-AB2D-2A0978BE05A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6086,21 +6329,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA6490E-A2D4-4F41-902E-623575711A1D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="44ef142f-35ce-48df-bc44-191ee5827fd0"/>
-    <ds:schemaRef ds:uri="a52c2c93-1616-4696-bc88-4a2586572708"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>